<commit_message>
Change title of ModelMusings readme.md
</commit_message>
<xml_diff>
--- a/TribalWater/TribalWaterStudyData.xlsx
+++ b/TribalWater/TribalWaterStudyData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20375"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20378"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCoding2\TribalWater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EE6D40F8-7096-4130-8872-9D728E834A0E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF98688-B95D-41E7-BD35-BE2F2DA0DF8F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5770" activeTab="2" xr2:uid="{CD95E5B1-F1F9-4E80-ABE3-16257A279FC8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5770" xr2:uid="{CD95E5B1-F1F9-4E80-ABE3-16257A279FC8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -59,7 +59,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -100,7 +100,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -944,7 +944,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EDD6961-BAAE-42EF-9ED2-97D5DAFE54FC}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -1024,7 +1024,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0A1F4B9-67B9-4E1A-A4AC-F4AFB957CCFF}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Add publications to md, update key ideas, com, add versions.
</commit_message>
<xml_diff>
--- a/TribalWater/TribalWaterStudyData.xlsx
+++ b/TribalWater/TribalWaterStudyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCoding2\TribalWater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CF98688-B95D-41E7-BD35-BE2F2DA0DF8F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C3F40B-DB1C-42CE-89C2-BBEBA2C7B82F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5770" xr2:uid="{CD95E5B1-F1F9-4E80-ABE3-16257A279FC8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5775" xr2:uid="{CD95E5B1-F1F9-4E80-ABE3-16257A279FC8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Upper Basin</t>
   </si>
@@ -51,6 +51,12 @@
   </si>
   <si>
     <t>Lower Basin Use from USBR Lower Basin Reports</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Rights perfected</t>
   </si>
 </sst>
 </file>
@@ -98,9 +104,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -942,32 +949,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EDD6961-BAAE-42EF-9ED2-97D5DAFE54FC}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -977,8 +988,12 @@
       <c r="C3" s="1">
         <v>952190</v>
       </c>
+      <c r="D3" s="2">
+        <f>SUM(B3:C3)</f>
+        <v>2012971</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -987,6 +1002,15 @@
       </c>
       <c r="C4" s="1">
         <v>22928</v>
+      </c>
+      <c r="D4" s="2">
+        <f>SUM(B4:C4)</f>
+        <v>785273</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1002,14 +1026,14 @@
       <selection activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
       <c r="P26" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>5</v>
       </c>
@@ -1028,9 +1052,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
Edit text in intro Model Guide
</commit_message>
<xml_diff>
--- a/TribalWater/TribalWaterStudyData.xlsx
+++ b/TribalWater/TribalWaterStudyData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Rosenberg\Work\USU\Research\ColoradoRiver\RCode\ColoradoRiverCoding2\TribalWater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01C3F40B-DB1C-42CE-89C2-BBEBA2C7B82F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8EB81C-5422-45B0-97FF-29B5EE610ADB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5775" xr2:uid="{CD95E5B1-F1F9-4E80-ABE3-16257A279FC8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="5780" xr2:uid="{CD95E5B1-F1F9-4E80-ABE3-16257A279FC8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -952,22 +952,22 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B3" sqref="B3:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -978,7 +978,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -993,7 +993,7 @@
         <v>2012971</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1008,7 +1008,7 @@
         <v>785273</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1026,14 +1026,14 @@
       <selection activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="26" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:16" x14ac:dyDescent="0.35">
       <c r="P26" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>5</v>
       </c>
@@ -1052,9 +1052,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>7</v>
       </c>

</xml_diff>